<commit_message>
Resolução de bug no banco
</commit_message>
<xml_diff>
--- a/temp/filtro_resultado.xlsx
+++ b/temp/filtro_resultado.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,45 +505,1334 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Cristian Silva Souza</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(27)99840-2562</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>05/05/2025</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>(27)99810-5464</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>45769</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Heittor Loriato Souza</t>
+        </is>
+      </c>
       <c r="E2" t="n">
-        <v>7</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
+        <v>14</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Gosta de jogos</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Alta</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Indicação</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>ctrlplay</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bernard</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>(27)99999-2408</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45761</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>9</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>CTRL+KIDS</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Não Feita</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Facebook</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Luzia</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>(27)99693-8513</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45761</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Gustavo</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>7</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Thayná</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>(27)99532-1738</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45757</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>9</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>MATUTINO</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kelly</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>(27)99267-7826</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45761</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>gosta de jogar</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Henrique</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>(27)99800-8586</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45759</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Bernardo</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>9</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>VESPERTINO disponível na seg a noite</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Eliane</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>(27)99245-4607</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>45729</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>7</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Queria aulas ao sabados</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Julio</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>(28)99905-9096</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Angela</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>(27)98846-5189</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>12</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sheila</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>(27)98146-5556</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Joga bastante</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Jéssica</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>(27)99708-0989</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>VESPERTINO</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Lavinya</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>(27)98816-4830</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Lavinya</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>17</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Curso de informatica</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>CTRL+YOUNG</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>(27)98853-3832</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>(27)99577-2157</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>45763</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>11</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Caio</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>(27)99285-6869</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>45763</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>5</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>(27)99741-8559</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>45766</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>(27)99760-9645</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>45769</v>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Jackeline</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>(27)99788-1919</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>45769</v>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Lidy</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>(27)99624-7100</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>45769</v>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="n">
+        <v>10</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Vitória</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>(27)99905-6780</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>45769</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Davi</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>7</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Não é alfabetizado</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Jackeline Salles</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>(27)98847-7535</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>45769</v>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>7</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Estuda a tarde</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>(27)99994-3500</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>45770</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Lucca</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>8</v>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Daniele</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>(27)98833-4829</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>45770</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Enzo</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>10</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Tiago</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>(27)99764-0144</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>45770</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Laura</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>8</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Ela gosta do Roblox</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>(27)99729-1612</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>45771</v>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>CTRL+KIDS</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Valéria</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>(27)98895-5231</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>45771</v>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Baixo</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Tamires</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>(27)99268-1081</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>45768</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Gabriel E Isabella</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>9</v>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Tereza</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>(27)99605-6561</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>45747</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Davi</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>10</v>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Médio</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>CTRL+TEENS</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Não Feita</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
         <is>
           <t>nao</t>
         </is>

</xml_diff>